<commit_message>
#change to version: - 2.1.10 Model - 0.1.23 RestServer - update the documentation
</commit_message>
<xml_diff>
--- a/Documentation/Credit-UI_Mapping.xlsx
+++ b/Documentation/Credit-UI_Mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6686550E-ECF0-43C5-9043-DE4E60F4C0AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263B222D-0794-4714-9EEA-4676541B0877}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="13" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <sheet name="Slide 20" sheetId="22" r:id="rId21"/>
     <sheet name="Slide 21" sheetId="23" r:id="rId22"/>
     <sheet name="Slide 22" sheetId="24" r:id="rId23"/>
-    <sheet name="Slide 27" sheetId="10" r:id="rId24"/>
+    <sheet name="Slide 23" sheetId="25" r:id="rId24"/>
+    <sheet name="Slide 24" sheetId="26" r:id="rId25"/>
+    <sheet name="Slide 27" sheetId="10" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="466">
   <si>
     <t>id</t>
   </si>
@@ -1634,12 +1636,256 @@
   <si>
     <t>22: Dlg 3.1 - Security Agreements I</t>
   </si>
+  <si>
+    <t>LoanAgreement.securityAgreements</t>
+  </si>
+  <si>
+    <t>Security agreement ComboBox</t>
+  </si>
+  <si>
+    <t>(SecurityAgreement) agreementDate</t>
+  </si>
+  <si>
+    <t>(SecurityAgreement) executionDate</t>
+  </si>
+  <si>
+    <t>Contracted Date</t>
+  </si>
+  <si>
+    <t>Executed Date</t>
+  </si>
+  <si>
+    <t>(SecurityAgreement) collAgreements</t>
+  </si>
+  <si>
+    <t>Collateral agreement ComboBox</t>
+  </si>
+  <si>
+    <t>Pledged from Date</t>
+  </si>
+  <si>
+    <t>Pledged to Date</t>
+  </si>
+  <si>
+    <t>limited to Checkbox</t>
+  </si>
+  <si>
+    <t>(CollateralAgreement) unlimitedYN</t>
+  </si>
+  <si>
+    <t>(CollateralAgreement) pledgedFrom</t>
+  </si>
+  <si>
+    <t>(CollateralAgreement) pledgedTo</t>
+  </si>
+  <si>
+    <t>Collaterals Listbox</t>
+  </si>
+  <si>
+    <t>Caption: SimpleClassName + " #" + collateral.id</t>
+  </si>
+  <si>
+    <t>(CollateralAgreement) collaterals.cashCollaterals
+AND
+(CollateralAgreement) collaterals.securityCollaterals</t>
+  </si>
+  <si>
+    <t>CashCollateral Custodian</t>
+  </si>
+  <si>
+    <t>CashCollateral Cash Account</t>
+  </si>
+  <si>
+    <t>CashCollateral Cash Accountholder</t>
+  </si>
+  <si>
+    <t>CashCollateral Cash entire account pledged</t>
+  </si>
+  <si>
+    <t>CashCollateral Cash pledged notional</t>
+  </si>
+  <si>
+    <t>CashCollateral Cash currency</t>
+  </si>
+  <si>
+    <t>CashCollateral Last Evaluation Evalution date</t>
+  </si>
+  <si>
+    <t>CashCollateral Last Evaluation value</t>
+  </si>
+  <si>
+    <t>CashCollateral Last Evaluation Currency</t>
+  </si>
+  <si>
+    <t>(CashCollateral) accountNumber</t>
+  </si>
+  <si>
+    <t>(Counterparty) name</t>
+  </si>
+  <si>
+    <t>(CashCollateral) amount.amount</t>
+  </si>
+  <si>
+    <t>(CashCollateral) amount.currencyIso</t>
+  </si>
+  <si>
+    <t>(CashCollateral) depositoryId -&gt; GET /counterparties/{id}</t>
+  </si>
+  <si>
+    <t>(CashCollateral) accountNumber -&gt; GET /accounts/{accNo} 
+From retrieved account get the mapping to the counterparties
+(Account) accountCounterparties.counterpartyId -&gt; GET /counterparties/{id}</t>
+  </si>
+  <si>
+    <t>23: Dlg 3.2 - Security Agreements II</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Custodian</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Evaluation value</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Evaluation Currency</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Evaluation Evalution date</t>
+  </si>
+  <si>
+    <t>(SecurityCollateral) depotNumber</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Securities Security Account</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Securities ISIN</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Securities Pledged notional</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Securities Currency</t>
+  </si>
+  <si>
+    <t>(SecurityCollateral) securityIsin</t>
+  </si>
+  <si>
+    <t>(SecurityCollateral) nominalValue</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Estimation Estimation date</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Estimation Value</t>
+  </si>
+  <si>
+    <t>SecurityCollateral Last Estimation Currency</t>
+  </si>
+  <si>
+    <t>24: Dlg 3.3 - Security Agreements III</t>
+  </si>
+  <si>
+    <t>(SecurityAgreement) guaranteeAgreements</t>
+  </si>
+  <si>
+    <t>Guarantee Agreements ComboBox</t>
+  </si>
+  <si>
+    <t>(GuaranteeAgreement) date</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement Contracted</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement Guarantor</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement Volume limited</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement Volume amount</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement Volume currency</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement irrevocable</t>
+  </si>
+  <si>
+    <t>Guarantee Agreement unconditional</t>
+  </si>
+  <si>
+    <t>(GuaranteeAgreement) kuendrechtGGYN</t>
+  </si>
+  <si>
+    <t>(GuaranteeAgreement) unbedingtYN</t>
+  </si>
+  <si>
+    <t>Calculated: IF amount = 0 then not limited</t>
+  </si>
+  <si>
+    <t>(GuaranteeAgreement) guaranteerId -&gt; GET /counterparties/{id}</t>
+  </si>
+  <si>
+    <t>(CollaterlAgreement) date</t>
+  </si>
+  <si>
+    <t>(CollateralAgreement) date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If (Collateral) amount.amount &lt;&gt; 0 then yes; else no</t>
+  </si>
+  <si>
+    <t>If (CashColleteral).depositoryId = 1 
+-&gt; (CashColleteral).accountNumber, LocalDate.now -&gt; GET accounts\{accountNumber}\balances\latest\{now} -&gt; (AccountBalance).date;
+Else (Collateral).date</t>
+  </si>
+  <si>
+    <t>If (CashColleteral).depositoryId = 1 
+-&gt; (CashColleteral).accountNumber, LocalDate.now -&gt; GET accounts\{accountNumber}\balances\latest\{now} -&gt; (AccountBalance).balance;
+Else (Collateral).amount.amount</t>
+  </si>
+  <si>
+    <t>If (CashColleteral).depositoryId = 1 
+-&gt; (CashColleteral).accountNumber, LocalDate.now -&gt; GET accounts\{accountNumber} -&gt; (Account).currencyIso;
+Else (Collateral).amount.currencyIso</t>
+  </si>
+  <si>
+    <t>(SecurityCollateral).securityIsin -&gt; GET /securities/{isin}</t>
+  </si>
+  <si>
+    <t>(Security).currencyIso</t>
+  </si>
+  <si>
+    <t>(SecurityCollateral).securityIsin, LocalDate.now -&gt; GET /securities/{isin}/price/{date}</t>
+  </si>
+  <si>
+    <t>(SecurityPrice).timeStamp</t>
+  </si>
+  <si>
+    <t>(SecurityPrice).amount.amount * (SecurityCollateral).nominalValue</t>
+  </si>
+  <si>
+    <t>(SecurityPrice).amount.currencyIso</t>
+  </si>
+  <si>
+    <t>(Collateral).date</t>
+  </si>
+  <si>
+    <t>(Collateral).amount.amount</t>
+  </si>
+  <si>
+    <t>(Collateral).amount.currencyIso</t>
+  </si>
+  <si>
+    <t>If no price is available</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1713,6 +1959,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1753,7 +2006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1816,6 +2069,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1828,16 +2119,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2137,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -2322,11 +2613,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2343,12 +2634,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2379,11 +2670,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2461,11 +2752,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2594,11 +2885,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2757,11 +3048,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2778,12 +3069,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2799,7 +3090,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,11 +3105,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2990,12 +3281,12 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -3006,11 +3297,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3119,7 +3410,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:D11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="131.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3135,11 +3426,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3186,7 +3477,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>326</v>
       </c>
@@ -3263,11 +3554,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3284,12 +3575,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -3338,7 +3629,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,11 +3644,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3457,11 +3748,11 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3571,7 +3862,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,11 +3877,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3711,11 +4002,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3870,7 +4161,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,11 +4177,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3929,10 +4220,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>289</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -3944,7 +4235,7 @@
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>375</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -3955,7 +4246,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>376</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -3966,10 +4257,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="29" t="s">
         <v>289</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -3980,7 +4271,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="29" t="s">
         <v>375</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -3988,7 +4279,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="29" t="s">
         <v>376</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -4061,17 +4352,18 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFC3A34-DC07-40CA-B04C-21620177527E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="123.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4079,11 +4371,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="45" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4100,47 +4392,164 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>393</v>
+      </c>
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="19"/>
+      <c r="B6" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="33" t="s">
+        <v>451</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
+      <c r="B10" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" t="s">
+        <v>403</v>
+      </c>
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="19"/>
+      <c r="A12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>406</v>
+      </c>
       <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="46"/>
+      <c r="C18" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="49"/>
+      <c r="C19" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="49"/>
+      <c r="C20" s="47" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>455</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4151,6 +4560,454 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EBCEE1-4339-4FC2-9CC5-E9644B0EE548}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>450</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" t="s">
+        <v>403</v>
+      </c>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>427</v>
+      </c>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>458</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="s">
+        <v>460</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="39" t="s">
+        <v>461</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="35" t="s">
+        <v>462</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>432</v>
+      </c>
+      <c r="D20" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="D21" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="35" t="s">
+        <v>464</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" t="s">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A956B028-69C3-486F-9255-6297C5219DE0}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" s="40"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>442</v>
+      </c>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="33" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DBC4C5-561E-48B8-A8CF-2584CEB3ADE9}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -4170,11 +5027,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4298,11 +5155,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4503,7 +5360,7 @@
       <c r="C18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="42" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4515,7 +5372,7 @@
       <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -4527,7 +5384,7 @@
       <c r="C20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="42" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4539,7 +5396,7 @@
       <c r="C21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -4565,7 +5422,7 @@
       <c r="C23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="42" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4577,7 +5434,7 @@
       <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -4624,11 +5481,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4780,25 +5637,25 @@
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="26"/>
+      <c r="D18" s="42"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="26"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="26"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -4810,13 +5667,13 @@
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -4855,11 +5712,11 @@
       <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -5077,11 +5934,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5284,11 +6141,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5381,11 +6238,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5469,11 +6326,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
#change to version: - 2.1.12 Model - 0.1.24 RestServer - update the documentation - https://github.com/Mangosoft-team/Demo/issues/34 - https://github.com/Mangosoft-team/Demo/issues/33 - https://github.com/Mangosoft-team/Demo/issues/26
</commit_message>
<xml_diff>
--- a/Documentation/Credit-UI_Mapping.xlsx
+++ b/Documentation/Credit-UI_Mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263B222D-0794-4714-9EEA-4676541B0877}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECA26B0-B5A7-4A69-A07D-906A994235C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="13" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -2107,6 +2107,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2119,16 +2129,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2613,11 +2613,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2634,12 +2634,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2670,11 +2670,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2752,11 +2752,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2885,11 +2885,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3048,11 +3048,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3069,12 +3069,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3089,8 +3089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26AE739-DE76-49AE-8B36-0CCB74A36021}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,11 +3105,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3297,11 +3297,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3426,11 +3426,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3554,11 +3554,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3575,12 +3575,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -3644,11 +3644,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3748,11 +3748,11 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3877,11 +3877,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4002,11 +4002,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4177,11 +4177,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4371,11 +4371,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4525,29 +4525,29 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="44" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="49"/>
-      <c r="C19" s="47" t="s">
+      <c r="B19" s="45"/>
+      <c r="C19" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="44" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
-      <c r="C20" s="47" t="s">
+      <c r="B20" s="45"/>
+      <c r="C20" s="43" t="s">
         <v>413</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="44" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4580,11 +4580,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>420</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4802,7 +4802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A956B028-69C3-486F-9255-6297C5219DE0}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -4818,11 +4818,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>435</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5027,11 +5027,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5155,11 +5155,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5360,7 +5360,7 @@
       <c r="C18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="46" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5372,7 +5372,7 @@
       <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="42"/>
+      <c r="D19" s="46"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -5384,7 +5384,7 @@
       <c r="C20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="46" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5396,7 +5396,7 @@
       <c r="C21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="42"/>
+      <c r="D21" s="46"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -5422,7 +5422,7 @@
       <c r="C23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="46" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5434,7 +5434,7 @@
       <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -5481,11 +5481,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5637,25 +5637,25 @@
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="42"/>
+      <c r="D18" s="46"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="42"/>
+      <c r="D19" s="46"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="42"/>
+      <c r="D20" s="46"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="42"/>
+      <c r="D21" s="46"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -5667,13 +5667,13 @@
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="42"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="42"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -5712,11 +5712,11 @@
       <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -5934,11 +5934,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -6141,11 +6141,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -6238,11 +6238,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -6326,11 +6326,11 @@
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>